<commit_message>
Stat screen added, graph screen's draft added
</commit_message>
<xml_diff>
--- a/src/brute_force/random_hitstand_results/random_hitstand_results.xlsx
+++ b/src/brute_force/random_hitstand_results/random_hitstand_results.xlsx
@@ -7,16 +7,17 @@
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="test0" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet name="test1" sheetId="2" state="visible" r:id="rId2"/>
-    <sheet name="test2" sheetId="3" state="visible" r:id="rId3"/>
-    <sheet name="test3" sheetId="4" state="visible" r:id="rId4"/>
-    <sheet name="test4" sheetId="5" state="visible" r:id="rId5"/>
-    <sheet name="test5" sheetId="6" state="visible" r:id="rId6"/>
-    <sheet name="test6" sheetId="7" state="visible" r:id="rId7"/>
-    <sheet name="test7" sheetId="8" state="visible" r:id="rId8"/>
-    <sheet name="test8" sheetId="9" state="visible" r:id="rId9"/>
-    <sheet name="test9" sheetId="10" state="visible" r:id="rId10"/>
+    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="test0" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="test1" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet name="test2" sheetId="4" state="visible" r:id="rId4"/>
+    <sheet name="test3" sheetId="5" state="visible" r:id="rId5"/>
+    <sheet name="test4" sheetId="6" state="visible" r:id="rId6"/>
+    <sheet name="test5" sheetId="7" state="visible" r:id="rId7"/>
+    <sheet name="test6" sheetId="8" state="visible" r:id="rId8"/>
+    <sheet name="test7" sheetId="9" state="visible" r:id="rId9"/>
+    <sheet name="test8" sheetId="10" state="visible" r:id="rId10"/>
+    <sheet name="test9" sheetId="11" state="visible" r:id="rId11"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -434,7 +435,25 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E21"/>
+  <dimension ref="A1:A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:E20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -472,19 +491,19 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>[Queen of Hearts, 6 of Hearts]</t>
+          <t>[6 of Clubs, 2 of Spades]</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>[2 of Clubs, 2 of Hearts, 1 of Diamonds, 3 of Spades]</t>
+          <t>[7 of Diamonds, 8 of Hearts, 5 of Clubs]</t>
         </is>
       </c>
       <c r="C2" t="n">
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="D2" t="n">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="E2" t="inlineStr">
         <is>
@@ -495,65 +514,65 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>[8 of Clubs, 10 of Spades, 2 of Spades]</t>
+          <t>[Queen of Hearts, King of Diamonds]</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>[1 of Hearts, 10 of Hearts]</t>
+          <t>[7 of Clubs, 3 of Clubs, Queen of Hearts]</t>
         </is>
       </c>
       <c r="C3" t="n">
         <v>20</v>
       </c>
       <c r="D3" t="n">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>Lose</t>
+          <t>Tie</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>[2 of Hearts, King of Diamonds]</t>
+          <t>[9 of Diamonds, King of Hearts]</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>[10 of Clubs, Jack of Diamonds]</t>
+          <t>[Jack of Clubs, 8 of Diamonds]</t>
         </is>
       </c>
       <c r="C4" t="n">
-        <v>12</v>
+        <v>19</v>
       </c>
       <c r="D4" t="n">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>Lose</t>
+          <t>Win</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>[5 of Spades, 5 of Hearts]</t>
+          <t>[5 of Diamonds, 10 of Spades]</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>[King of Hearts, 7 of Clubs]</t>
+          <t>[1 of Spades, 1 of Hearts, 1 of Diamonds, 6 of Diamonds]</t>
         </is>
       </c>
       <c r="C5" t="n">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="D5" t="n">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="E5" t="inlineStr">
         <is>
@@ -564,19 +583,19 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>[Queen of Spades, 10 of Diamonds, King of Hearts]</t>
+          <t>[6 of Clubs, Jack of Hearts]</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>[9 of Spades, 3 of Spades, 8 of Diamonds]</t>
+          <t>[8 of Spades, Queen of Spades]</t>
         </is>
       </c>
       <c r="C6" t="n">
-        <v>30</v>
+        <v>16</v>
       </c>
       <c r="D6" t="n">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="E6" t="inlineStr">
         <is>
@@ -587,42 +606,42 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>[Jack of Hearts, 5 of Hearts, 1 of Clubs]</t>
+          <t>[King of Spades, 7 of Spades]</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>[9 of Hearts, 4 of Hearts, King of Spades]</t>
+          <t>[Queen of Diamonds, 10 of Spades]</t>
         </is>
       </c>
       <c r="C7" t="n">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="D7" t="n">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>Win</t>
+          <t>Lose</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>[2 of Diamonds, 8 of Diamonds]</t>
+          <t>[6 of Spades, 8 of Spades]</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>[Jack of Diamonds, 1 of Clubs]</t>
+          <t>[2 of Diamonds, 7 of Clubs, Queen of Diamonds]</t>
         </is>
       </c>
       <c r="C8" t="n">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="D8" t="n">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="E8" t="inlineStr">
         <is>
@@ -633,42 +652,42 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>[4 of Clubs, 5 of Spades, 6 of Diamonds]</t>
+          <t>[10 of Hearts, 1 of Spades, 3 of Hearts, 2 of Diamonds, 5 of Hearts]</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>[2 of Diamonds, 4 of Diamonds, 7 of Spades, 7 of Hearts]</t>
+          <t>[Jack of Diamonds, 9 of Diamonds]</t>
         </is>
       </c>
       <c r="C9" t="n">
-        <v>15</v>
+        <v>21</v>
       </c>
       <c r="D9" t="n">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>Lose</t>
+          <t>Win</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>[9 of Diamonds, 9 of Hearts]</t>
+          <t>[9 of Hearts, 7 of Hearts]</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>[9 of Clubs, King of Diamonds]</t>
+          <t>[King of Clubs, Jack of Diamonds]</t>
         </is>
       </c>
       <c r="C10" t="n">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="D10" t="n">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="E10" t="inlineStr">
         <is>
@@ -679,42 +698,42 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>[4 of Diamonds, 3 of Clubs]</t>
+          <t>[Jack of Clubs, 2 of Spades]</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>[4 of Clubs, Jack of Clubs, 7 of Hearts]</t>
+          <t>[5 of Spades, 8 of Clubs, 10 of Clubs]</t>
         </is>
       </c>
       <c r="C11" t="n">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="D11" t="n">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>Lose</t>
+          <t>Win</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>[Queen of Clubs, 8 of Hearts]</t>
+          <t>[9 of Spades, 4 of Spades]</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>[6 of Diamonds, 1 of Spades]</t>
+          <t>[8 of Clubs, 3 of Diamonds, 4 of Hearts, 9 of Spades]</t>
         </is>
       </c>
       <c r="C12" t="n">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="D12" t="n">
-        <v>17</v>
+        <v>24</v>
       </c>
       <c r="E12" t="inlineStr">
         <is>
@@ -725,88 +744,88 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>[Jack of Hearts, Jack of Clubs, 8 of Spades]</t>
+          <t>[5 of Spades, King of Diamonds, 3 of Hearts]</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>[5 of Diamonds, 5 of Clubs, 7 of Spades]</t>
+          <t>[2 of Clubs, 7 of Spades, 9 of Hearts]</t>
         </is>
       </c>
       <c r="C13" t="n">
-        <v>28</v>
+        <v>18</v>
       </c>
       <c r="D13" t="n">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>Lose</t>
+          <t>Tie</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>[8 of Hearts, 5 of Clubs]</t>
+          <t>[1 of Diamonds, 2 of Hearts]</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>[Queen of Clubs, Queen of Hearts]</t>
+          <t>[4 of Clubs, 7 of Diamonds, 4 of Clubs, King of Clubs]</t>
         </is>
       </c>
       <c r="C14" t="n">
         <v>13</v>
       </c>
       <c r="D14" t="n">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>Lose</t>
+          <t>Win</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>[Queen of Spades, 3 of Clubs]</t>
+          <t>[4 of Diamonds, 6 of Hearts]</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>[9 of Spades, King of Spades]</t>
+          <t>[9 of Clubs, 3 of Clubs, 3 of Spades, 10 of Hearts]</t>
         </is>
       </c>
       <c r="C15" t="n">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="D15" t="n">
-        <v>19</v>
+        <v>25</v>
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>Lose</t>
+          <t>Win</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>[6 of Hearts, 10 of Clubs, Jack of Spades]</t>
+          <t>[Queen of Clubs, 3 of Diamonds, Jack of Spades, 5 of Clubs]</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>[Queen of Diamonds, 3 of Diamonds, 4 of Hearts]</t>
+          <t>[8 of Hearts, 6 of Hearts, 4 of Diamonds]</t>
         </is>
       </c>
       <c r="C16" t="n">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="D16" t="n">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="E16" t="inlineStr">
         <is>
@@ -817,16 +836,16 @@
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>[4 of Spades, 8 of Spades, Queen of Diamonds]</t>
+          <t>[2 of Clubs, 4 of Spades]</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>[7 of Diamonds, 3 of Hearts, 7 of Diamonds]</t>
+          <t>[1 of Clubs, 6 of Spades]</t>
         </is>
       </c>
       <c r="C17" t="n">
-        <v>22</v>
+        <v>6</v>
       </c>
       <c r="D17" t="n">
         <v>17</v>
@@ -840,19 +859,19 @@
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>[6 of Spades, 2 of Clubs, 1 of Hearts, 5 of Diamonds]</t>
+          <t>[2 of Hearts, Queen of Spades, 5 of Diamonds, 1 of Hearts, King of Spades, 10 of Diamonds]</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>[10 of Spades, 9 of Clubs]</t>
+          <t>[5 of Hearts, 10 of Diamonds, 7 of Hearts]</t>
         </is>
       </c>
       <c r="C18" t="n">
-        <v>14</v>
+        <v>38</v>
       </c>
       <c r="D18" t="n">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="E18" t="inlineStr">
         <is>
@@ -863,19 +882,19 @@
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>[10 of Diamonds, 6 of Clubs, 3 of Hearts, 6 of Clubs]</t>
+          <t>[1 of Clubs, Jack of Hearts, 8 of Diamonds, Jack of Spades]</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>[King of Clubs, 7 of Clubs]</t>
+          <t>[4 of Hearts, 10 of Clubs, 9 of Clubs]</t>
         </is>
       </c>
       <c r="C19" t="n">
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="D19" t="n">
-        <v>17</v>
+        <v>23</v>
       </c>
       <c r="E19" t="inlineStr">
         <is>
@@ -883,42 +902,13 @@
         </is>
       </c>
     </row>
-    <row r="20">
-      <c r="A20" t="inlineStr">
-        <is>
-          <t>[8 of Clubs, 4 of Spades, 1 of Spades, 2 of Spades, King of Clubs]</t>
-        </is>
-      </c>
-      <c r="B20" t="inlineStr">
-        <is>
-          <t>[10 of Hearts, 1 of Diamonds]</t>
-        </is>
-      </c>
-      <c r="C20" t="n">
-        <v>25</v>
-      </c>
-      <c r="D20" t="n">
-        <v>21</v>
-      </c>
-      <c r="E20" t="inlineStr">
-        <is>
-          <t>Lose</t>
-        </is>
-      </c>
-    </row>
-    <row r="21">
-      <c r="A21" t="inlineStr"/>
-      <c r="B21" t="inlineStr"/>
-      <c r="C21" t="inlineStr"/>
-      <c r="D21" t="inlineStr"/>
-      <c r="E21" t="inlineStr"/>
-    </row>
+    <row r="20"/>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -962,42 +952,42 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>[2 of Hearts, 5 of Hearts]</t>
+          <t>[9 of Hearts, King of Diamonds]</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>[5 of Clubs, 6 of Diamonds, 8 of Spades]</t>
+          <t>[King of Spades, 4 of Spades, Queen of Clubs]</t>
         </is>
       </c>
       <c r="C2" t="n">
-        <v>7</v>
+        <v>19</v>
       </c>
       <c r="D2" t="n">
-        <v>19</v>
+        <v>24</v>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>Lose</t>
+          <t>Win</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>[8 of Hearts, 4 of Hearts]</t>
+          <t>[10 of Spades, 9 of Spades]</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>[10 of Hearts, 8 of Spades]</t>
+          <t>[5 of Diamonds, 3 of Clubs, 3 of Spades, 1 of Diamonds, 8 of Hearts]</t>
         </is>
       </c>
       <c r="C3" t="n">
-        <v>12</v>
+        <v>19</v>
       </c>
       <c r="D3" t="n">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="E3" t="inlineStr">
         <is>
@@ -1008,19 +998,19 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>[8 of Clubs, 8 of Clubs, 2 of Diamonds]</t>
+          <t>[4 of Hearts, Jack of Diamonds]</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>[3 of Spades, Queen of Spades, 7 of Hearts]</t>
+          <t>[Queen of Spades, 4 of Diamonds, 7 of Spades]</t>
         </is>
       </c>
       <c r="C4" t="n">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="D4" t="n">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="E4" t="inlineStr">
         <is>
@@ -1031,19 +1021,19 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>[1 of Spades, 3 of Hearts, 5 of Spades, Jack of Clubs, 5 of Diamonds, King of Clubs]</t>
+          <t>[King of Clubs, 2 of Clubs, 9 of Hearts, 2 of Diamonds]</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>[3 of Diamonds, 6 of Hearts, King of Diamonds]</t>
+          <t>[Queen of Clubs, 6 of Diamonds, 10 of Diamonds]</t>
         </is>
       </c>
       <c r="C5" t="n">
-        <v>34</v>
+        <v>23</v>
       </c>
       <c r="D5" t="n">
-        <v>19</v>
+        <v>26</v>
       </c>
       <c r="E5" t="inlineStr">
         <is>
@@ -1054,157 +1044,157 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>[7 of Diamonds, Jack of Diamonds, 3 of Clubs]</t>
+          <t>[4 of Diamonds, Queen of Hearts, 9 of Diamonds, King of Hearts]</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>[Queen of Diamonds, 2 of Spades, 5 of Clubs]</t>
+          <t>[2 of Hearts, 5 of Clubs, King of Spades]</t>
         </is>
       </c>
       <c r="C6" t="n">
-        <v>20</v>
+        <v>33</v>
       </c>
       <c r="D6" t="n">
         <v>17</v>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>Win</t>
+          <t>Lose</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>[3 of Clubs, 4 of Clubs]</t>
+          <t>[1 of Hearts, 7 of Hearts, Queen of Diamonds]</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>[Queen of Clubs, 7 of Clubs]</t>
+          <t>[10 of Spades, 5 of Spades, 3 of Diamonds]</t>
         </is>
       </c>
       <c r="C7" t="n">
-        <v>7</v>
+        <v>18</v>
       </c>
       <c r="D7" t="n">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>Lose</t>
+          <t>Tie</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>[9 of Clubs, 6 of Diamonds, 7 of Clubs]</t>
+          <t>[4 of Hearts, King of Diamonds, 5 of Clubs]</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>[5 of Hearts, King of Spades, Jack of Clubs]</t>
+          <t>[7 of Clubs, Queen of Diamonds]</t>
         </is>
       </c>
       <c r="C8" t="n">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="D8" t="n">
-        <v>25</v>
+        <v>17</v>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>Lose</t>
+          <t>Win</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>[5 of Diamonds, Jack of Spades, 10 of Diamonds]</t>
+          <t>[1 of Clubs, 8 of Spades]</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>[4 of Diamonds, Queen of Diamonds, Queen of Hearts]</t>
+          <t>[3 of Spades, 3 of Clubs, 3 of Hearts, 3 of Diamonds, 7 of Diamonds]</t>
         </is>
       </c>
       <c r="C9" t="n">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="D9" t="n">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>Lose</t>
+          <t>Tie</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>[King of Hearts, 6 of Spades, 4 of Diamonds]</t>
+          <t>[2 of Spades, 8 of Diamonds]</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>[8 of Diamonds, Queen of Clubs]</t>
+          <t>[Jack of Hearts, 7 of Diamonds]</t>
         </is>
       </c>
       <c r="C10" t="n">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="D10" t="n">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>Win</t>
+          <t>Lose</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>[8 of Diamonds, King of Hearts]</t>
+          <t>[8 of Clubs, 1 of Hearts]</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>[10 of Hearts, 9 of Spades]</t>
+          <t>[10 of Diamonds, 9 of Clubs]</t>
         </is>
       </c>
       <c r="C11" t="n">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="D11" t="n">
         <v>19</v>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>Lose</t>
+          <t>Tie</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>[1 of Clubs, 1 of Spades]</t>
+          <t>[2 of Diamonds, Jack of Hearts, 1 of Diamonds, Queen of Hearts, 5 of Spades, 10 of Hearts, 8 of Diamonds]</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>[7 of Spades, 4 of Clubs, Jack of Hearts]</t>
+          <t>[Jack of Clubs, 3 of Hearts, 9 of Diamonds]</t>
         </is>
       </c>
       <c r="C12" t="n">
-        <v>12</v>
+        <v>46</v>
       </c>
       <c r="D12" t="n">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="E12" t="inlineStr">
         <is>
@@ -1215,88 +1205,88 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>[4 of Spades, 9 of Clubs, 10 of Clubs, Queen of Hearts, 9 of Diamonds, King of Clubs, 1 of Diamonds, 9 of Diamonds]</t>
+          <t>[6 of Clubs, 5 of Diamonds]</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>[10 of Spades, 2 of Spades, Queen of Spades]</t>
+          <t>[2 of Hearts, 8 of Spades, 5 of Hearts, 9 of Clubs]</t>
         </is>
       </c>
       <c r="C13" t="n">
-        <v>62</v>
+        <v>11</v>
       </c>
       <c r="D13" t="n">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>Lose</t>
+          <t>Win</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>[4 of Spades, 5 of Spades]</t>
+          <t>[Jack of Clubs, 2 of Spades]</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>[2 of Diamonds, 10 of Diamonds, Jack of Hearts]</t>
+          <t>[Jack of Spades, 5 of Hearts, 1 of Clubs, 2 of Clubs]</t>
         </is>
       </c>
       <c r="C14" t="n">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="D14" t="n">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>Win</t>
+          <t>Lose</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>[2 of Hearts, 1 of Hearts, 4 of Hearts, Jack of Diamonds, 3 of Spades]</t>
+          <t>[6 of Diamonds, 6 of Clubs, 6 of Spades]</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>[6 of Clubs, King of Spades, 2 of Clubs]</t>
+          <t>[8 of Hearts, 4 of Spades, 4 of Clubs, 4 of Clubs]</t>
         </is>
       </c>
       <c r="C15" t="n">
+        <v>18</v>
+      </c>
+      <c r="D15" t="n">
         <v>20</v>
       </c>
-      <c r="D15" t="n">
-        <v>18</v>
-      </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>Win</t>
+          <t>Lose</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>[Jack of Spades, 10 of Clubs, 1 of Hearts, 1 of Diamonds]</t>
+          <t>[Queen of Spades, 9 of Spades, 7 of Spades, 6 of Hearts, 10 of Clubs]</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>[7 of Diamonds, 7 of Spades, 9 of Hearts]</t>
+          <t>[Jack of Diamonds, 7 of Clubs]</t>
         </is>
       </c>
       <c r="C16" t="n">
-        <v>32</v>
+        <v>42</v>
       </c>
       <c r="D16" t="n">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="E16" t="inlineStr">
         <is>
@@ -1307,32 +1297,32 @@
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>[3 of Hearts, 6 of Hearts, 8 of Hearts, 9 of Hearts, 10 of Spades]</t>
+          <t>[10 of Clubs, 1 of Spades]</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>[6 of Spades, 1 of Clubs]</t>
+          <t>[6 of Hearts, King of Hearts, 7 of Hearts]</t>
         </is>
       </c>
       <c r="C17" t="n">
-        <v>36</v>
+        <v>21</v>
       </c>
       <c r="D17" t="n">
-        <v>17</v>
+        <v>23</v>
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>Lose</t>
+          <t>Win</t>
         </is>
       </c>
     </row>
     <row r="18">
-      <c r="E18" t="inlineStr">
-        <is>
-          <t>% 25.00</t>
-        </is>
-      </c>
+      <c r="A18" t="inlineStr"/>
+      <c r="B18" t="inlineStr"/>
+      <c r="C18" t="inlineStr"/>
+      <c r="D18" t="inlineStr"/>
+      <c r="E18" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -1345,7 +1335,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E18"/>
+  <dimension ref="A1:E17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1383,19 +1373,19 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>[2 of Hearts, 5 of Hearts]</t>
+          <t>[2 of Diamonds, 4 of Spades, 5 of Diamonds]</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>[5 of Clubs, 6 of Diamonds, 8 of Spades]</t>
+          <t>[Jack of Hearts, Queen of Spades]</t>
         </is>
       </c>
       <c r="C2" t="n">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="D2" t="n">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="E2" t="inlineStr">
         <is>
@@ -1406,19 +1396,19 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>[8 of Hearts, 4 of Hearts]</t>
+          <t>[5 of Clubs, Jack of Hearts]</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>[10 of Hearts, 8 of Spades]</t>
+          <t>[Queen of Clubs, King of Clubs]</t>
         </is>
       </c>
       <c r="C3" t="n">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="D3" t="n">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="E3" t="inlineStr">
         <is>
@@ -1429,65 +1419,65 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>[8 of Clubs, 8 of Clubs, 2 of Diamonds]</t>
+          <t>[1 of Diamonds, 1 of Hearts]</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>[3 of Spades, Queen of Spades, 7 of Hearts]</t>
+          <t>[6 of Spades, Queen of Clubs, 7 of Hearts]</t>
         </is>
       </c>
       <c r="C4" t="n">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="D4" t="n">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>Lose</t>
+          <t>Win</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>[1 of Spades, 3 of Hearts, 5 of Spades, Jack of Clubs, 5 of Diamonds, King of Clubs]</t>
+          <t>[8 of Hearts, 10 of Diamonds]</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>[3 of Diamonds, 6 of Hearts, King of Diamonds]</t>
+          <t>[2 of Clubs, Jack of Diamonds, 2 of Diamonds, King of Hearts]</t>
         </is>
       </c>
       <c r="C5" t="n">
-        <v>34</v>
+        <v>18</v>
       </c>
       <c r="D5" t="n">
-        <v>19</v>
+        <v>24</v>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>Lose</t>
+          <t>Win</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>[7 of Diamonds, Jack of Diamonds, 3 of Clubs]</t>
+          <t>[9 of Spades, 6 of Diamonds]</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>[Queen of Diamonds, 2 of Spades, 5 of Clubs]</t>
+          <t>[7 of Clubs, 9 of Hearts, 8 of Spades]</t>
         </is>
       </c>
       <c r="C6" t="n">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="D6" t="n">
-        <v>17</v>
+        <v>24</v>
       </c>
       <c r="E6" t="inlineStr">
         <is>
@@ -1498,19 +1488,19 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>[3 of Clubs, 4 of Clubs]</t>
+          <t>[9 of Diamonds, 5 of Spades, Queen of Hearts, 3 of Diamonds]</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>[Queen of Clubs, 7 of Clubs]</t>
+          <t>[Queen of Diamonds, 1 of Clubs]</t>
         </is>
       </c>
       <c r="C7" t="n">
-        <v>7</v>
+        <v>27</v>
       </c>
       <c r="D7" t="n">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="E7" t="inlineStr">
         <is>
@@ -1521,19 +1511,19 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>[9 of Clubs, 6 of Diamonds, 7 of Clubs]</t>
+          <t>[Queen of Diamonds, King of Diamonds, 3 of Clubs]</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>[5 of Hearts, King of Spades, Jack of Clubs]</t>
+          <t>[3 of Diamonds, 2 of Hearts, 7 of Spades, 8 of Clubs]</t>
         </is>
       </c>
       <c r="C8" t="n">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D8" t="n">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="E8" t="inlineStr">
         <is>
@@ -1544,19 +1534,19 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>[5 of Diamonds, Jack of Spades, 10 of Diamonds]</t>
+          <t>[6 of Clubs, 3 of Hearts, 4 of Diamonds, King of Spades]</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>[4 of Diamonds, Queen of Diamonds, Queen of Hearts]</t>
+          <t>[4 of Diamonds, Jack of Clubs, 7 of Diamonds]</t>
         </is>
       </c>
       <c r="C9" t="n">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="D9" t="n">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="E9" t="inlineStr">
         <is>
@@ -1567,42 +1557,42 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>[King of Hearts, 6 of Spades, 4 of Diamonds]</t>
+          <t>[9 of Clubs, 5 of Hearts]</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>[8 of Diamonds, Queen of Clubs]</t>
+          <t>[8 of Hearts, King of Clubs]</t>
         </is>
       </c>
       <c r="C10" t="n">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="D10" t="n">
         <v>18</v>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>Win</t>
+          <t>Lose</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>[8 of Diamonds, King of Hearts]</t>
+          <t>[8 of Diamonds, 9 of Clubs]</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>[10 of Hearts, 9 of Spades]</t>
+          <t>[King of Hearts, Jack of Spades]</t>
         </is>
       </c>
       <c r="C11" t="n">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D11" t="n">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="E11" t="inlineStr">
         <is>
@@ -1613,19 +1603,19 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>[1 of Clubs, 1 of Spades]</t>
+          <t>[10 of Clubs, 9 of Diamonds, 9 of Hearts, 2 of Hearts, 10 of Hearts]</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>[7 of Spades, 4 of Clubs, Jack of Hearts]</t>
+          <t>[5 of Spades, 5 of Clubs, 5 of Diamonds, 10 of Clubs]</t>
         </is>
       </c>
       <c r="C12" t="n">
-        <v>12</v>
+        <v>40</v>
       </c>
       <c r="D12" t="n">
-        <v>21</v>
+        <v>25</v>
       </c>
       <c r="E12" t="inlineStr">
         <is>
@@ -1636,42 +1626,42 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>[4 of Spades, 9 of Clubs, 10 of Clubs, Queen of Hearts, 9 of Diamonds, King of Clubs, 1 of Diamonds, 9 of Diamonds]</t>
+          <t>[9 of Spades, 1 of Hearts]</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>[10 of Spades, 2 of Spades, Queen of Spades]</t>
+          <t>[Jack of Diamonds, 7 of Spades]</t>
         </is>
       </c>
       <c r="C13" t="n">
-        <v>62</v>
+        <v>20</v>
       </c>
       <c r="D13" t="n">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>Lose</t>
+          <t>Win</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>[4 of Spades, 5 of Spades]</t>
+          <t>[4 of Clubs, 6 of Clubs, 1 of Diamonds]</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>[2 of Diamonds, 10 of Diamonds, Jack of Hearts]</t>
+          <t>[1 of Spades, 8 of Clubs]</t>
         </is>
       </c>
       <c r="C14" t="n">
-        <v>9</v>
+        <v>21</v>
       </c>
       <c r="D14" t="n">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="E14" t="inlineStr">
         <is>
@@ -1682,42 +1672,42 @@
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>[2 of Hearts, 1 of Hearts, 4 of Hearts, Jack of Diamonds, 3 of Spades]</t>
+          <t>[8 of Diamonds, 2 of Clubs, 4 of Clubs, Queen of Spades]</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>[6 of Clubs, King of Spades, 2 of Clubs]</t>
+          <t>[3 of Hearts, 2 of Spades, 4 of Hearts, 7 of Clubs, 8 of Spades]</t>
         </is>
       </c>
       <c r="C15" t="n">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="D15" t="n">
-        <v>18</v>
+        <v>24</v>
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>Win</t>
+          <t>Lose</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>[Jack of Spades, 10 of Clubs, 1 of Hearts, 1 of Diamonds]</t>
+          <t>[10 of Diamonds, Jack of Spades, Jack of Clubs, Queen of Hearts]</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>[7 of Diamonds, 7 of Spades, 9 of Hearts]</t>
+          <t>[3 of Spades, 3 of Clubs, 6 of Hearts, King of Diamonds]</t>
         </is>
       </c>
       <c r="C16" t="n">
-        <v>32</v>
+        <v>40</v>
       </c>
       <c r="D16" t="n">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E16" t="inlineStr">
         <is>
@@ -1728,16 +1718,16 @@
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>[3 of Hearts, 6 of Hearts, 8 of Hearts, 9 of Hearts, 10 of Spades]</t>
+          <t>[10 of Hearts, 1 of Clubs, 4 of Spades, 6 of Spades, King of Spades]</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>[6 of Spades, 1 of Clubs]</t>
+          <t>[7 of Diamonds, 10 of Spades]</t>
         </is>
       </c>
       <c r="C17" t="n">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="D17" t="n">
         <v>17</v>
@@ -1745,13 +1735,6 @@
       <c r="E17" t="inlineStr">
         <is>
           <t>Lose</t>
-        </is>
-      </c>
-    </row>
-    <row r="18">
-      <c r="E18" t="inlineStr">
-        <is>
-          <t>% 25.00</t>
         </is>
       </c>
     </row>
@@ -1804,19 +1787,19 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>[2 of Hearts, 5 of Hearts]</t>
+          <t>[10 of Spades, 7 of Clubs]</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>[5 of Clubs, 6 of Diamonds, 8 of Spades]</t>
+          <t>[1 of Clubs, 1 of Diamonds, 8 of Hearts]</t>
         </is>
       </c>
       <c r="C2" t="n">
-        <v>7</v>
+        <v>17</v>
       </c>
       <c r="D2" t="n">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="E2" t="inlineStr">
         <is>
@@ -1827,19 +1810,19 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>[8 of Hearts, 4 of Hearts]</t>
+          <t>[King of Clubs, 7 of Clubs, Jack of Diamonds, 5 of Hearts, Jack of Spades, 10 of Hearts]</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>[10 of Hearts, 8 of Spades]</t>
+          <t>[7 of Spades, 9 of Diamonds, King of Diamonds]</t>
         </is>
       </c>
       <c r="C3" t="n">
-        <v>12</v>
+        <v>52</v>
       </c>
       <c r="D3" t="n">
-        <v>18</v>
+        <v>26</v>
       </c>
       <c r="E3" t="inlineStr">
         <is>
@@ -1850,19 +1833,19 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>[8 of Clubs, 8 of Clubs, 2 of Diamonds]</t>
+          <t>[9 of Hearts, 5 of Diamonds, King of Spades]</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>[3 of Spades, Queen of Spades, 7 of Hearts]</t>
+          <t>[10 of Diamonds, 3 of Diamonds, 4 of Clubs]</t>
         </is>
       </c>
       <c r="C4" t="n">
-        <v>18</v>
+        <v>24</v>
       </c>
       <c r="D4" t="n">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="E4" t="inlineStr">
         <is>
@@ -1873,65 +1856,65 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>[1 of Spades, 3 of Hearts, 5 of Spades, Jack of Clubs, 5 of Diamonds, King of Clubs]</t>
+          <t>[King of Hearts, 10 of Hearts]</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>[3 of Diamonds, 6 of Hearts, King of Diamonds]</t>
+          <t>[Queen of Diamonds, 6 of Diamonds, 3 of Hearts]</t>
         </is>
       </c>
       <c r="C5" t="n">
-        <v>34</v>
+        <v>20</v>
       </c>
       <c r="D5" t="n">
         <v>19</v>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>Lose</t>
+          <t>Win</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>[7 of Diamonds, Jack of Diamonds, 3 of Clubs]</t>
+          <t>[3 of Spades, Queen of Hearts, 10 of Spades]</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>[Queen of Diamonds, 2 of Spades, 5 of Clubs]</t>
+          <t>[2 of Diamonds, 4 of Diamonds, 2 of Spades, 8 of Clubs, 8 of Diamonds]</t>
         </is>
       </c>
       <c r="C6" t="n">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="D6" t="n">
-        <v>17</v>
+        <v>24</v>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>Win</t>
+          <t>Lose</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>[3 of Clubs, 4 of Clubs]</t>
+          <t>[Queen of Clubs, 3 of Spades]</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>[Queen of Clubs, 7 of Clubs]</t>
+          <t>[9 of Spades, 4 of Spades, 8 of Clubs]</t>
         </is>
       </c>
       <c r="C7" t="n">
-        <v>7</v>
+        <v>13</v>
       </c>
       <c r="D7" t="n">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="E7" t="inlineStr">
         <is>
@@ -1942,19 +1925,19 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>[9 of Clubs, 6 of Diamonds, 7 of Clubs]</t>
+          <t>[5 of Clubs, 2 of Clubs, 5 of Clubs]</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>[5 of Hearts, King of Spades, Jack of Clubs]</t>
+          <t>[1 of Hearts, 9 of Clubs]</t>
         </is>
       </c>
       <c r="C8" t="n">
-        <v>22</v>
+        <v>12</v>
       </c>
       <c r="D8" t="n">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="E8" t="inlineStr">
         <is>
@@ -1965,19 +1948,19 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>[5 of Diamonds, Jack of Spades, 10 of Diamonds]</t>
+          <t>[10 of Clubs, 5 of Spades]</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>[4 of Diamonds, Queen of Diamonds, Queen of Hearts]</t>
+          <t>[1 of Spades, 8 of Hearts]</t>
         </is>
       </c>
       <c r="C9" t="n">
-        <v>25</v>
+        <v>15</v>
       </c>
       <c r="D9" t="n">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="E9" t="inlineStr">
         <is>
@@ -1988,19 +1971,19 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>[King of Hearts, 6 of Spades, 4 of Diamonds]</t>
+          <t>[7 of Hearts, Queen of Clubs]</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>[8 of Diamonds, Queen of Clubs]</t>
+          <t>[9 of Diamonds, 3 of Clubs, 1 of Spades, 2 of Hearts, 1 of Hearts, King of Clubs]</t>
         </is>
       </c>
       <c r="C10" t="n">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="D10" t="n">
-        <v>18</v>
+        <v>26</v>
       </c>
       <c r="E10" t="inlineStr">
         <is>
@@ -2011,19 +1994,19 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>[8 of Diamonds, King of Hearts]</t>
+          <t>[Queen of Hearts, Jack of Hearts]</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>[10 of Hearts, 9 of Spades]</t>
+          <t>[1 of Clubs, Jack of Clubs]</t>
         </is>
       </c>
       <c r="C11" t="n">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="D11" t="n">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="E11" t="inlineStr">
         <is>
@@ -2034,19 +2017,19 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>[1 of Clubs, 1 of Spades]</t>
+          <t>[2 of Clubs, 5 of Spades, 8 of Spades, Jack of Diamonds]</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>[7 of Spades, 4 of Clubs, Jack of Hearts]</t>
+          <t>[6 of Hearts, 3 of Diamonds, 3 of Hearts, Queen of Diamonds]</t>
         </is>
       </c>
       <c r="C12" t="n">
-        <v>12</v>
+        <v>25</v>
       </c>
       <c r="D12" t="n">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="E12" t="inlineStr">
         <is>
@@ -2057,19 +2040,19 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>[4 of Spades, 9 of Clubs, 10 of Clubs, Queen of Hearts, 9 of Diamonds, King of Clubs, 1 of Diamonds, 9 of Diamonds]</t>
+          <t>[7 of Diamonds, 4 of Diamonds]</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>[10 of Spades, 2 of Spades, Queen of Spades]</t>
+          <t>[King of Hearts, 9 of Clubs]</t>
         </is>
       </c>
       <c r="C13" t="n">
-        <v>62</v>
+        <v>11</v>
       </c>
       <c r="D13" t="n">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="E13" t="inlineStr">
         <is>
@@ -2080,88 +2063,88 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>[4 of Spades, 5 of Spades]</t>
+          <t>[4 of Hearts, 6 of Spades, 8 of Diamonds]</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>[2 of Diamonds, 10 of Diamonds, Jack of Hearts]</t>
+          <t>[9 of Spades, 1 of Diamonds]</t>
         </is>
       </c>
       <c r="C14" t="n">
-        <v>9</v>
+        <v>18</v>
       </c>
       <c r="D14" t="n">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>Win</t>
+          <t>Lose</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>[2 of Hearts, 1 of Hearts, 4 of Hearts, Jack of Diamonds, 3 of Spades]</t>
+          <t>[6 of Clubs, 9 of Hearts]</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>[6 of Clubs, King of Spades, 2 of Clubs]</t>
+          <t>[2 of Hearts, 7 of Hearts, 4 of Spades, 6 of Hearts]</t>
         </is>
       </c>
       <c r="C15" t="n">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="D15" t="n">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>Win</t>
+          <t>Lose</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>[Jack of Spades, 10 of Clubs, 1 of Hearts, 1 of Diamonds]</t>
+          <t>[4 of Hearts, 4 of Clubs, 7 of Spades]</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>[7 of Diamonds, 7 of Spades, 9 of Hearts]</t>
+          <t>[Jack of Spades, 2 of Spades, Jack of Clubs]</t>
         </is>
       </c>
       <c r="C16" t="n">
-        <v>32</v>
+        <v>15</v>
       </c>
       <c r="D16" t="n">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>Lose</t>
+          <t>Win</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>[3 of Hearts, 6 of Hearts, 8 of Hearts, 9 of Hearts, 10 of Spades]</t>
+          <t>[King of Spades, 5 of Diamonds, 7 of Diamonds]</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>[6 of Spades, 1 of Clubs]</t>
+          <t>[Queen of Spades, 3 of Clubs, 10 of Diamonds]</t>
         </is>
       </c>
       <c r="C17" t="n">
-        <v>36</v>
+        <v>22</v>
       </c>
       <c r="D17" t="n">
-        <v>17</v>
+        <v>23</v>
       </c>
       <c r="E17" t="inlineStr">
         <is>
@@ -2170,9 +2153,25 @@
       </c>
     </row>
     <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>[Jack of Hearts, 5 of Hearts, 10 of Clubs]</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>[6 of Spades, 6 of Diamonds, 6 of Clubs]</t>
+        </is>
+      </c>
+      <c r="C18" t="n">
+        <v>25</v>
+      </c>
+      <c r="D18" t="n">
+        <v>18</v>
+      </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>% 25.00</t>
+          <t>Lose</t>
         </is>
       </c>
     </row>
@@ -2187,7 +2186,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E18"/>
+  <dimension ref="A1:E16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2225,19 +2224,19 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>[2 of Hearts, 5 of Hearts]</t>
+          <t>[1 of Hearts, 5 of Diamonds, 10 of Clubs, Queen of Diamonds, 10 of Diamonds]</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>[5 of Clubs, 6 of Diamonds, 8 of Spades]</t>
+          <t>[Queen of Spades, 2 of Diamonds, 5 of Clubs]</t>
         </is>
       </c>
       <c r="C2" t="n">
-        <v>7</v>
+        <v>36</v>
       </c>
       <c r="D2" t="n">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="E2" t="inlineStr">
         <is>
@@ -2248,19 +2247,19 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>[8 of Hearts, 4 of Hearts]</t>
+          <t>[9 of Spades, 3 of Clubs]</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>[10 of Hearts, 8 of Spades]</t>
+          <t>[6 of Diamonds, 7 of Clubs, 7 of Spades]</t>
         </is>
       </c>
       <c r="C3" t="n">
         <v>12</v>
       </c>
       <c r="D3" t="n">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="E3" t="inlineStr">
         <is>
@@ -2271,42 +2270,42 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>[8 of Clubs, 8 of Clubs, 2 of Diamonds]</t>
+          <t>[Queen of Clubs, 7 of Spades]</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>[3 of Spades, Queen of Spades, 7 of Hearts]</t>
+          <t>[6 of Spades, 6 of Hearts, King of Spades]</t>
         </is>
       </c>
       <c r="C4" t="n">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D4" t="n">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>Lose</t>
+          <t>Win</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>[1 of Spades, 3 of Hearts, 5 of Spades, Jack of Clubs, 5 of Diamonds, King of Clubs]</t>
+          <t>[Jack of Hearts, 3 of Clubs, Queen of Diamonds, 3 of Hearts, 3 of Spades]</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>[3 of Diamonds, 6 of Hearts, King of Diamonds]</t>
+          <t>[1 of Clubs, Queen of Hearts]</t>
         </is>
       </c>
       <c r="C5" t="n">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="D5" t="n">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="E5" t="inlineStr">
         <is>
@@ -2317,39 +2316,39 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>[7 of Diamonds, Jack of Diamonds, 3 of Clubs]</t>
+          <t>[1 of Diamonds, 6 of Diamonds, 4 of Diamonds, 8 of Diamonds, 3 of Diamonds, Jack of Diamonds]</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>[Queen of Diamonds, 2 of Spades, 5 of Clubs]</t>
+          <t>[5 of Diamonds, 9 of Spades, 9 of Diamonds]</t>
         </is>
       </c>
       <c r="C6" t="n">
-        <v>20</v>
+        <v>32</v>
       </c>
       <c r="D6" t="n">
-        <v>17</v>
+        <v>23</v>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>Win</t>
+          <t>Lose</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>[3 of Clubs, 4 of Clubs]</t>
+          <t>[1 of Spades, 8 of Clubs, 9 of Clubs, 8 of Spades, King of Diamonds]</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>[Queen of Clubs, 7 of Clubs]</t>
+          <t>[Jack of Clubs, 2 of Spades, 5 of Spades]</t>
         </is>
       </c>
       <c r="C7" t="n">
-        <v>7</v>
+        <v>36</v>
       </c>
       <c r="D7" t="n">
         <v>17</v>
@@ -2363,19 +2362,19 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>[9 of Clubs, 6 of Diamonds, 7 of Clubs]</t>
+          <t>[5 of Hearts, 1 of Hearts, 9 of Hearts]</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>[5 of Hearts, King of Spades, Jack of Clubs]</t>
+          <t>[Queen of Clubs, 2 of Hearts, 1 of Spades, 5 of Clubs]</t>
         </is>
       </c>
       <c r="C8" t="n">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="D8" t="n">
-        <v>25</v>
+        <v>18</v>
       </c>
       <c r="E8" t="inlineStr">
         <is>
@@ -2386,19 +2385,19 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>[5 of Diamonds, Jack of Spades, 10 of Diamonds]</t>
+          <t>[7 of Diamonds, King of Hearts]</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>[4 of Diamonds, Queen of Diamonds, Queen of Hearts]</t>
+          <t>[4 of Clubs, 7 of Diamonds, 2 of Hearts, 2 of Diamonds, 4 of Hearts]</t>
         </is>
       </c>
       <c r="C9" t="n">
-        <v>25</v>
+        <v>17</v>
       </c>
       <c r="D9" t="n">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="E9" t="inlineStr">
         <is>
@@ -2409,42 +2408,42 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>[King of Hearts, 6 of Spades, 4 of Diamonds]</t>
+          <t>[6 of Clubs, King of Clubs, 10 of Hearts]</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>[8 of Diamonds, Queen of Clubs]</t>
+          <t>[3 of Hearts, 9 of Hearts, 7 of Clubs]</t>
         </is>
       </c>
       <c r="C10" t="n">
-        <v>20</v>
+        <v>26</v>
       </c>
       <c r="D10" t="n">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>Win</t>
+          <t>Lose</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>[8 of Diamonds, King of Hearts]</t>
+          <t>[8 of Spades, 4 of Clubs]</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>[10 of Hearts, 9 of Spades]</t>
+          <t>[3 of Spades, 2 of Clubs, 4 of Diamonds, 3 of Diamonds, 5 of Spades]</t>
         </is>
       </c>
       <c r="C11" t="n">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="D11" t="n">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="E11" t="inlineStr">
         <is>
@@ -2455,42 +2454,42 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>[1 of Clubs, 1 of Spades]</t>
+          <t>[Queen of Hearts, Jack of Spades]</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>[7 of Spades, 4 of Clubs, Jack of Hearts]</t>
+          <t>[7 of Hearts, Jack of Clubs]</t>
         </is>
       </c>
       <c r="C12" t="n">
-        <v>12</v>
+        <v>20</v>
       </c>
       <c r="D12" t="n">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>Lose</t>
+          <t>Win</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>[4 of Spades, 9 of Clubs, 10 of Clubs, Queen of Hearts, 9 of Diamonds, King of Clubs, 1 of Diamonds, 9 of Diamonds]</t>
+          <t>[10 of Spades, Jack of Hearts, 6 of Clubs]</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>[10 of Spades, 2 of Spades, Queen of Spades]</t>
+          <t>[King of Clubs, 8 of Clubs]</t>
         </is>
       </c>
       <c r="C13" t="n">
-        <v>62</v>
+        <v>26</v>
       </c>
       <c r="D13" t="n">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="E13" t="inlineStr">
         <is>
@@ -2501,19 +2500,19 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>[4 of Spades, 5 of Spades]</t>
+          <t>[8 of Hearts, King of Hearts]</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>[2 of Diamonds, 10 of Diamonds, Jack of Hearts]</t>
+          <t>[2 of Clubs, 4 of Hearts, 4 of Spades, 6 of Spades, 8 of Diamonds]</t>
         </is>
       </c>
       <c r="C14" t="n">
-        <v>9</v>
+        <v>18</v>
       </c>
       <c r="D14" t="n">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="E14" t="inlineStr">
         <is>
@@ -2524,76 +2523,46 @@
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>[2 of Hearts, 1 of Hearts, 4 of Hearts, Jack of Diamonds, 3 of Spades]</t>
+          <t>[6 of Hearts, 1 of Diamonds]</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>[6 of Clubs, King of Spades, 2 of Clubs]</t>
+          <t>[8 of Hearts, 9 of Clubs]</t>
         </is>
       </c>
       <c r="C15" t="n">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="D15" t="n">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>Win</t>
+          <t>Tie</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>[Jack of Spades, 10 of Clubs, 1 of Hearts, 1 of Diamonds]</t>
+          <t>[10 of Diamonds, 10 of Hearts]</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>[7 of Diamonds, 7 of Spades, 9 of Hearts]</t>
+          <t>[5 of Hearts, 9 of Diamonds, 2 of Spades, Jack of Diamonds]</t>
         </is>
       </c>
       <c r="C16" t="n">
-        <v>32</v>
+        <v>20</v>
       </c>
       <c r="D16" t="n">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>Lose</t>
-        </is>
-      </c>
-    </row>
-    <row r="17">
-      <c r="A17" t="inlineStr">
-        <is>
-          <t>[3 of Hearts, 6 of Hearts, 8 of Hearts, 9 of Hearts, 10 of Spades]</t>
-        </is>
-      </c>
-      <c r="B17" t="inlineStr">
-        <is>
-          <t>[6 of Spades, 1 of Clubs]</t>
-        </is>
-      </c>
-      <c r="C17" t="n">
-        <v>36</v>
-      </c>
-      <c r="D17" t="n">
-        <v>17</v>
-      </c>
-      <c r="E17" t="inlineStr">
-        <is>
-          <t>Lose</t>
-        </is>
-      </c>
-    </row>
-    <row r="18">
-      <c r="E18" t="inlineStr">
-        <is>
-          <t>% 25.00</t>
+          <t>Win</t>
         </is>
       </c>
     </row>
@@ -2646,16 +2615,16 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>[2 of Hearts, 5 of Hearts]</t>
+          <t>[10 of Hearts, 6 of Hearts, King of Spades, King of Clubs]</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>[5 of Clubs, 6 of Diamonds, 8 of Spades]</t>
+          <t>[2 of Hearts, 7 of Hearts, Queen of Hearts]</t>
         </is>
       </c>
       <c r="C2" t="n">
-        <v>7</v>
+        <v>36</v>
       </c>
       <c r="D2" t="n">
         <v>19</v>
@@ -2669,42 +2638,42 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>[8 of Hearts, 4 of Hearts]</t>
+          <t>[6 of Hearts, Queen of Diamonds]</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>[10 of Hearts, 8 of Spades]</t>
+          <t>[Jack of Clubs, 3 of Diamonds, 9 of Spades]</t>
         </is>
       </c>
       <c r="C3" t="n">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="D3" t="n">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>Lose</t>
+          <t>Win</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>[8 of Clubs, 8 of Clubs, 2 of Diamonds]</t>
+          <t>[8 of Clubs, 2 of Clubs]</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>[3 of Spades, Queen of Spades, 7 of Hearts]</t>
+          <t>[Queen of Spades, 1 of Hearts]</t>
         </is>
       </c>
       <c r="C4" t="n">
-        <v>18</v>
+        <v>10</v>
       </c>
       <c r="D4" t="n">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="E4" t="inlineStr">
         <is>
@@ -2715,19 +2684,19 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>[1 of Spades, 3 of Hearts, 5 of Spades, Jack of Clubs, 5 of Diamonds, King of Clubs]</t>
+          <t>[3 of Hearts, 8 of Diamonds]</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>[3 of Diamonds, 6 of Hearts, King of Diamonds]</t>
+          <t>[Queen of Diamonds, 8 of Hearts]</t>
         </is>
       </c>
       <c r="C5" t="n">
-        <v>34</v>
+        <v>11</v>
       </c>
       <c r="D5" t="n">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E5" t="inlineStr">
         <is>
@@ -2738,42 +2707,42 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>[7 of Diamonds, Jack of Diamonds, 3 of Clubs]</t>
+          <t>[4 of Spades, 3 of Hearts, 6 of Clubs]</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>[Queen of Diamonds, 2 of Spades, 5 of Clubs]</t>
+          <t>[Jack of Clubs, Jack of Spades]</t>
         </is>
       </c>
       <c r="C6" t="n">
+        <v>13</v>
+      </c>
+      <c r="D6" t="n">
         <v>20</v>
       </c>
-      <c r="D6" t="n">
-        <v>17</v>
-      </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>Win</t>
+          <t>Lose</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>[3 of Clubs, 4 of Clubs]</t>
+          <t>[5 of Hearts, 1 of Diamonds]</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>[Queen of Clubs, 7 of Clubs]</t>
+          <t>[7 of Diamonds, 1 of Hearts]</t>
         </is>
       </c>
       <c r="C7" t="n">
-        <v>7</v>
+        <v>16</v>
       </c>
       <c r="D7" t="n">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="E7" t="inlineStr">
         <is>
@@ -2784,85 +2753,85 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>[9 of Clubs, 6 of Diamonds, 7 of Clubs]</t>
+          <t>[3 of Clubs, 1 of Diamonds]</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>[5 of Hearts, King of Spades, Jack of Clubs]</t>
+          <t>[2 of Clubs, Queen of Hearts, 4 of Clubs, King of Diamonds]</t>
         </is>
       </c>
       <c r="C8" t="n">
-        <v>22</v>
+        <v>14</v>
       </c>
       <c r="D8" t="n">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>Lose</t>
+          <t>Win</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>[5 of Diamonds, Jack of Spades, 10 of Diamonds]</t>
+          <t>[4 of Diamonds, King of Hearts, 7 of Spades]</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>[4 of Diamonds, Queen of Diamonds, Queen of Hearts]</t>
+          <t>[4 of Hearts, 1 of Clubs, 9 of Spades, Jack of Hearts]</t>
         </is>
       </c>
       <c r="C9" t="n">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="D9" t="n">
         <v>24</v>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>Lose</t>
+          <t>Win</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>[King of Hearts, 6 of Spades, 4 of Diamonds]</t>
+          <t>[5 of Spades, 5 of Clubs, 9 of Hearts]</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>[8 of Diamonds, Queen of Clubs]</t>
+          <t>[1 of Spades, 2 of Spades, 7 of Clubs]</t>
         </is>
       </c>
       <c r="C10" t="n">
+        <v>19</v>
+      </c>
+      <c r="D10" t="n">
         <v>20</v>
       </c>
-      <c r="D10" t="n">
-        <v>18</v>
-      </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>Win</t>
+          <t>Lose</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>[8 of Diamonds, King of Hearts]</t>
+          <t>[10 of Spades, 4 of Hearts]</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>[10 of Hearts, 9 of Spades]</t>
+          <t>[9 of Hearts, Jack of Spades]</t>
         </is>
       </c>
       <c r="C11" t="n">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="D11" t="n">
         <v>19</v>
@@ -2876,19 +2845,19 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>[1 of Clubs, 1 of Spades]</t>
+          <t>[6 of Spades, 2 of Diamonds, 2 of Spades, 4 of Spades]</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>[7 of Spades, 4 of Clubs, Jack of Hearts]</t>
+          <t>[3 of Clubs, 4 of Diamonds, King of Diamonds]</t>
         </is>
       </c>
       <c r="C12" t="n">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="D12" t="n">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="E12" t="inlineStr">
         <is>
@@ -2899,19 +2868,19 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>[4 of Spades, 9 of Clubs, 10 of Clubs, Queen of Hearts, 9 of Diamonds, King of Clubs, 1 of Diamonds, 9 of Diamonds]</t>
+          <t>[8 of Hearts, 9 of Clubs]</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>[10 of Spades, 2 of Spades, Queen of Spades]</t>
+          <t>[1 of Clubs, 10 of Hearts]</t>
         </is>
       </c>
       <c r="C13" t="n">
-        <v>62</v>
+        <v>17</v>
       </c>
       <c r="D13" t="n">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E13" t="inlineStr">
         <is>
@@ -2922,19 +2891,19 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>[4 of Spades, 5 of Spades]</t>
+          <t>[3 of Diamonds, 5 of Diamonds, 2 of Diamonds]</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>[2 of Diamonds, 10 of Diamonds, Jack of Hearts]</t>
+          <t>[8 of Clubs, 7 of Diamonds, Jack of Diamonds]</t>
         </is>
       </c>
       <c r="C14" t="n">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D14" t="n">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="E14" t="inlineStr">
         <is>
@@ -2945,39 +2914,39 @@
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>[2 of Hearts, 1 of Hearts, 4 of Hearts, Jack of Diamonds, 3 of Spades]</t>
+          <t>[3 of Spades, 9 of Diamonds, 8 of Diamonds, 10 of Diamonds]</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>[6 of Clubs, King of Spades, 2 of Clubs]</t>
+          <t>[Queen of Spades, 5 of Clubs, 3 of Spades]</t>
         </is>
       </c>
       <c r="C15" t="n">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="D15" t="n">
         <v>18</v>
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>Win</t>
+          <t>Lose</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>[Jack of Spades, 10 of Clubs, 1 of Hearts, 1 of Diamonds]</t>
+          <t>[10 of Clubs, King of Spades, 8 of Spades, 4 of Clubs, 9 of Clubs]</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>[7 of Diamonds, 7 of Spades, 9 of Hearts]</t>
+          <t>[5 of Hearts, 6 of Diamonds, 2 of Hearts, Queen of Clubs]</t>
         </is>
       </c>
       <c r="C16" t="n">
-        <v>32</v>
+        <v>41</v>
       </c>
       <c r="D16" t="n">
         <v>23</v>
@@ -2991,19 +2960,19 @@
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>[3 of Hearts, 6 of Hearts, 8 of Hearts, 9 of Hearts, 10 of Spades]</t>
+          <t>[10 of Spades, 7 of Spades, 1 of Spades]</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>[6 of Spades, 1 of Clubs]</t>
+          <t>[9 of Diamonds, 10 of Diamonds]</t>
         </is>
       </c>
       <c r="C17" t="n">
-        <v>36</v>
+        <v>18</v>
       </c>
       <c r="D17" t="n">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="E17" t="inlineStr">
         <is>
@@ -3012,9 +2981,25 @@
       </c>
     </row>
     <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>[10 of Clubs, King of Hearts, 8 of Spades, 6 of Clubs]</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>[Jack of Hearts, 6 of Spades, 5 of Spades]</t>
+        </is>
+      </c>
+      <c r="C18" t="n">
+        <v>34</v>
+      </c>
+      <c r="D18" t="n">
+        <v>21</v>
+      </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>% 25.00</t>
+          <t>Lose</t>
         </is>
       </c>
     </row>
@@ -3029,7 +3014,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E18"/>
+  <dimension ref="A1:E19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3067,39 +3052,39 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>[2 of Hearts, 5 of Hearts]</t>
+          <t>[4 of Diamonds, Jack of Diamonds, 6 of Hearts]</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>[5 of Clubs, 6 of Diamonds, 8 of Spades]</t>
+          <t>[7 of Spades, 1 of Diamonds]</t>
         </is>
       </c>
       <c r="C2" t="n">
-        <v>7</v>
+        <v>20</v>
       </c>
       <c r="D2" t="n">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>Lose</t>
+          <t>Win</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>[8 of Hearts, 4 of Hearts]</t>
+          <t>[8 of Hearts, 10 of Clubs, 4 of Spades, Jack of Diamonds]</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>[10 of Hearts, 8 of Spades]</t>
+          <t>[Queen of Diamonds, 8 of Diamonds]</t>
         </is>
       </c>
       <c r="C3" t="n">
-        <v>12</v>
+        <v>32</v>
       </c>
       <c r="D3" t="n">
         <v>18</v>
@@ -3113,19 +3098,19 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>[8 of Clubs, 8 of Clubs, 2 of Diamonds]</t>
+          <t>[Jack of Spades, 8 of Spades]</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>[3 of Spades, Queen of Spades, 7 of Hearts]</t>
+          <t>[8 of Diamonds, 1 of Spades]</t>
         </is>
       </c>
       <c r="C4" t="n">
         <v>18</v>
       </c>
       <c r="D4" t="n">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E4" t="inlineStr">
         <is>
@@ -3136,19 +3121,19 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>[1 of Spades, 3 of Hearts, 5 of Spades, Jack of Clubs, 5 of Diamonds, King of Clubs]</t>
+          <t>[6 of Spades, King of Spades, Queen of Clubs, 8 of Clubs, 3 of Spades]</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>[3 of Diamonds, 6 of Hearts, King of Diamonds]</t>
+          <t>[2 of Hearts, 1 of Diamonds, 7 of Clubs]</t>
         </is>
       </c>
       <c r="C5" t="n">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="D5" t="n">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="E5" t="inlineStr">
         <is>
@@ -3159,42 +3144,42 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>[7 of Diamonds, Jack of Diamonds, 3 of Clubs]</t>
+          <t>[5 of Diamonds, Queen of Clubs, King of Spades, 2 of Diamonds]</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>[Queen of Diamonds, 2 of Spades, 5 of Clubs]</t>
+          <t>[9 of Spades, 8 of Clubs]</t>
         </is>
       </c>
       <c r="C6" t="n">
-        <v>20</v>
+        <v>27</v>
       </c>
       <c r="D6" t="n">
         <v>17</v>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>Win</t>
+          <t>Lose</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>[3 of Clubs, 4 of Clubs]</t>
+          <t>[7 of Spades, 6 of Spades]</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>[Queen of Clubs, 7 of Clubs]</t>
+          <t>[3 of Hearts, 2 of Hearts, 10 of Spades, 5 of Spades]</t>
         </is>
       </c>
       <c r="C7" t="n">
-        <v>7</v>
+        <v>13</v>
       </c>
       <c r="D7" t="n">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="E7" t="inlineStr">
         <is>
@@ -3205,19 +3190,19 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>[9 of Clubs, 6 of Diamonds, 7 of Clubs]</t>
+          <t>[7 of Hearts, 10 of Diamonds, 9 of Hearts]</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>[5 of Hearts, King of Spades, Jack of Clubs]</t>
+          <t>[8 of Spades, King of Clubs]</t>
         </is>
       </c>
       <c r="C8" t="n">
-        <v>22</v>
+        <v>26</v>
       </c>
       <c r="D8" t="n">
-        <v>25</v>
+        <v>18</v>
       </c>
       <c r="E8" t="inlineStr">
         <is>
@@ -3228,19 +3213,19 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>[5 of Diamonds, Jack of Spades, 10 of Diamonds]</t>
+          <t>[Queen of Spades, 3 of Diamonds]</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>[4 of Diamonds, Queen of Diamonds, Queen of Hearts]</t>
+          <t>[5 of Diamonds, Queen of Hearts, 4 of Hearts]</t>
         </is>
       </c>
       <c r="C9" t="n">
-        <v>25</v>
+        <v>13</v>
       </c>
       <c r="D9" t="n">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="E9" t="inlineStr">
         <is>
@@ -3251,65 +3236,65 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>[King of Hearts, 6 of Spades, 4 of Diamonds]</t>
+          <t>[7 of Hearts, Jack of Hearts]</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>[8 of Diamonds, Queen of Clubs]</t>
+          <t>[7 of Diamonds, King of Hearts]</t>
         </is>
       </c>
       <c r="C10" t="n">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="D10" t="n">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>Win</t>
+          <t>Tie</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>[8 of Diamonds, King of Hearts]</t>
+          <t>[Jack of Hearts, King of Hearts]</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>[10 of Hearts, 9 of Spades]</t>
+          <t>[7 of Clubs, 4 of Spades, 4 of Clubs, 10 of Diamonds]</t>
         </is>
       </c>
       <c r="C11" t="n">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="D11" t="n">
-        <v>19</v>
+        <v>25</v>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>Lose</t>
+          <t>Win</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>[1 of Clubs, 1 of Spades]</t>
+          <t>[Jack of Clubs, 2 of Clubs, King of Clubs]</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>[7 of Spades, 4 of Clubs, Jack of Hearts]</t>
+          <t>[9 of Spades, 5 of Clubs, King of Diamonds]</t>
         </is>
       </c>
       <c r="C12" t="n">
-        <v>12</v>
+        <v>22</v>
       </c>
       <c r="D12" t="n">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="E12" t="inlineStr">
         <is>
@@ -3320,19 +3305,19 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>[4 of Spades, 9 of Clubs, 10 of Clubs, Queen of Hearts, 9 of Diamonds, King of Clubs, 1 of Diamonds, 9 of Diamonds]</t>
+          <t>[3 of Clubs, 9 of Hearts, 2 of Spades]</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>[10 of Spades, 2 of Spades, Queen of Spades]</t>
+          <t>[10 of Hearts, 10 of Spades]</t>
         </is>
       </c>
       <c r="C13" t="n">
-        <v>62</v>
+        <v>14</v>
       </c>
       <c r="D13" t="n">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="E13" t="inlineStr">
         <is>
@@ -3343,65 +3328,65 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>[4 of Spades, 5 of Spades]</t>
+          <t>[4 of Hearts, 7 of Diamonds]</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>[2 of Diamonds, 10 of Diamonds, Jack of Hearts]</t>
+          <t>[2 of Diamonds, 3 of Hearts, King of Diamonds, 5 of Hearts]</t>
         </is>
       </c>
       <c r="C14" t="n">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="D14" t="n">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>Win</t>
+          <t>Lose</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>[2 of Hearts, 1 of Hearts, 4 of Hearts, Jack of Diamonds, 3 of Spades]</t>
+          <t>[Jack of Spades, 9 of Diamonds, 8 of Hearts]</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>[6 of Clubs, King of Spades, 2 of Clubs]</t>
+          <t>[4 of Clubs, Queen of Hearts, 6 of Diamonds]</t>
         </is>
       </c>
       <c r="C15" t="n">
+        <v>27</v>
+      </c>
+      <c r="D15" t="n">
         <v>20</v>
       </c>
-      <c r="D15" t="n">
-        <v>18</v>
-      </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>Win</t>
+          <t>Lose</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>[Jack of Spades, 10 of Clubs, 1 of Hearts, 1 of Diamonds]</t>
+          <t>[6 of Diamonds, 10 of Hearts]</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>[7 of Diamonds, 7 of Spades, 9 of Hearts]</t>
+          <t>[Jack of Clubs, 1 of Hearts]</t>
         </is>
       </c>
       <c r="C16" t="n">
-        <v>32</v>
+        <v>16</v>
       </c>
       <c r="D16" t="n">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="E16" t="inlineStr">
         <is>
@@ -3412,30 +3397,69 @@
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>[3 of Hearts, 6 of Hearts, 8 of Hearts, 9 of Hearts, 10 of Spades]</t>
+          <t>[1 of Clubs, 1 of Hearts, 2 of Spades]</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>[6 of Spades, 1 of Clubs]</t>
+          <t>[1 of Clubs, 3 of Spades, 6 of Clubs]</t>
         </is>
       </c>
       <c r="C17" t="n">
-        <v>36</v>
+        <v>14</v>
       </c>
       <c r="D17" t="n">
+        <v>20</v>
+      </c>
+      <c r="E17" t="inlineStr">
+        <is>
+          <t>Lose</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>[4 of Diamonds, 9 of Diamonds]</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>[1 of Spades, Queen of Diamonds]</t>
+        </is>
+      </c>
+      <c r="C18" t="n">
+        <v>13</v>
+      </c>
+      <c r="D18" t="n">
+        <v>21</v>
+      </c>
+      <c r="E18" t="inlineStr">
+        <is>
+          <t>Lose</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>[3 of Diamonds, 9 of Clubs]</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>[9 of Clubs, 5 of Clubs, 3 of Clubs]</t>
+        </is>
+      </c>
+      <c r="C19" t="n">
+        <v>12</v>
+      </c>
+      <c r="D19" t="n">
         <v>17</v>
       </c>
-      <c r="E17" t="inlineStr">
-        <is>
-          <t>Lose</t>
-        </is>
-      </c>
-    </row>
-    <row r="18">
-      <c r="E18" t="inlineStr">
-        <is>
-          <t>% 25.00</t>
+      <c r="E19" t="inlineStr">
+        <is>
+          <t>Lose</t>
         </is>
       </c>
     </row>
@@ -3450,7 +3474,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E18"/>
+  <dimension ref="A1:E19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3488,19 +3512,19 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>[2 of Hearts, 5 of Hearts]</t>
+          <t>[King of Diamonds, 5 of Hearts]</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>[5 of Clubs, 6 of Diamonds, 8 of Spades]</t>
+          <t>[1 of Spades, Queen of Diamonds]</t>
         </is>
       </c>
       <c r="C2" t="n">
-        <v>7</v>
+        <v>15</v>
       </c>
       <c r="D2" t="n">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="E2" t="inlineStr">
         <is>
@@ -3511,39 +3535,39 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>[8 of Hearts, 4 of Hearts]</t>
+          <t>[6 of Diamonds, 2 of Clubs, 1 of Diamonds]</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>[10 of Hearts, 8 of Spades]</t>
+          <t>[1 of Clubs, 7 of Hearts]</t>
         </is>
       </c>
       <c r="C3" t="n">
-        <v>12</v>
+        <v>19</v>
       </c>
       <c r="D3" t="n">
         <v>18</v>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>Lose</t>
+          <t>Win</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>[8 of Clubs, 8 of Clubs, 2 of Diamonds]</t>
+          <t>[10 of Clubs, 4 of Clubs]</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>[3 of Spades, Queen of Spades, 7 of Hearts]</t>
+          <t>[3 of Diamonds, 2 of Hearts, 7 of Spades, 8 of Diamonds]</t>
         </is>
       </c>
       <c r="C4" t="n">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="D4" t="n">
         <v>20</v>
@@ -3557,16 +3581,16 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>[1 of Spades, 3 of Hearts, 5 of Spades, Jack of Clubs, 5 of Diamonds, King of Clubs]</t>
+          <t>[6 of Diamonds, 4 of Spades]</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>[3 of Diamonds, 6 of Hearts, King of Diamonds]</t>
+          <t>[7 of Clubs, 2 of Hearts, Jack of Hearts]</t>
         </is>
       </c>
       <c r="C5" t="n">
-        <v>34</v>
+        <v>10</v>
       </c>
       <c r="D5" t="n">
         <v>19</v>
@@ -3580,42 +3604,42 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>[7 of Diamonds, Jack of Diamonds, 3 of Clubs]</t>
+          <t>[9 of Diamonds, 5 of Diamonds, 2 of Clubs, King of Spades, Jack of Clubs]</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>[Queen of Diamonds, 2 of Spades, 5 of Clubs]</t>
+          <t>[2 of Spades, 1 of Spades, 3 of Spades, 4 of Diamonds]</t>
         </is>
       </c>
       <c r="C6" t="n">
+        <v>36</v>
+      </c>
+      <c r="D6" t="n">
         <v>20</v>
       </c>
-      <c r="D6" t="n">
-        <v>17</v>
-      </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>Win</t>
+          <t>Lose</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>[3 of Clubs, 4 of Clubs]</t>
+          <t>[Jack of Hearts, 7 of Diamonds, 10 of Hearts, Jack of Clubs]</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>[Queen of Clubs, 7 of Clubs]</t>
+          <t>[King of Clubs, 4 of Clubs, 8 of Clubs]</t>
         </is>
       </c>
       <c r="C7" t="n">
-        <v>7</v>
+        <v>37</v>
       </c>
       <c r="D7" t="n">
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="E7" t="inlineStr">
         <is>
@@ -3626,19 +3650,19 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>[9 of Clubs, 6 of Diamonds, 7 of Clubs]</t>
+          <t>[5 of Spades, 4 of Diamonds, Queen of Spades, 3 of Diamonds]</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>[5 of Hearts, King of Spades, Jack of Clubs]</t>
+          <t>[2 of Diamonds, 7 of Hearts, 6 of Hearts, 2 of Diamonds]</t>
         </is>
       </c>
       <c r="C8" t="n">
         <v>22</v>
       </c>
       <c r="D8" t="n">
-        <v>25</v>
+        <v>17</v>
       </c>
       <c r="E8" t="inlineStr">
         <is>
@@ -3649,88 +3673,88 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>[5 of Diamonds, Jack of Spades, 10 of Diamonds]</t>
+          <t>[King of Diamonds, 5 of Clubs, 4 of Spades]</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>[4 of Diamonds, Queen of Diamonds, Queen of Hearts]</t>
+          <t>[9 of Hearts, 6 of Clubs, King of Clubs]</t>
         </is>
       </c>
       <c r="C9" t="n">
+        <v>19</v>
+      </c>
+      <c r="D9" t="n">
         <v>25</v>
       </c>
-      <c r="D9" t="n">
-        <v>24</v>
-      </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>Lose</t>
+          <t>Win</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>[King of Hearts, 6 of Spades, 4 of Diamonds]</t>
+          <t>[King of Hearts, 8 of Spades]</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>[8 of Diamonds, Queen of Clubs]</t>
+          <t>[9 of Hearts, 9 of Spades]</t>
         </is>
       </c>
       <c r="C10" t="n">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="D10" t="n">
         <v>18</v>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>Win</t>
+          <t>Tie</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>[8 of Diamonds, King of Hearts]</t>
+          <t>[1 of Hearts, 3 of Clubs, 3 of Spades]</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>[10 of Hearts, 9 of Spades]</t>
+          <t>[6 of Hearts, 7 of Diamonds, 10 of Clubs]</t>
         </is>
       </c>
       <c r="C11" t="n">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D11" t="n">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>Lose</t>
+          <t>Win</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>[1 of Clubs, 1 of Spades]</t>
+          <t>[9 of Diamonds, 6 of Spades]</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>[7 of Spades, 4 of Clubs, Jack of Hearts]</t>
+          <t>[9 of Spades, Jack of Diamonds]</t>
         </is>
       </c>
       <c r="C12" t="n">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="D12" t="n">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="E12" t="inlineStr">
         <is>
@@ -3741,19 +3765,19 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>[4 of Spades, 9 of Clubs, 10 of Clubs, Queen of Hearts, 9 of Diamonds, King of Clubs, 1 of Diamonds, 9 of Diamonds]</t>
+          <t>[8 of Diamonds, Queen of Clubs, 6 of Spades]</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>[10 of Spades, 2 of Spades, Queen of Spades]</t>
+          <t>[8 of Hearts, 10 of Spades]</t>
         </is>
       </c>
       <c r="C13" t="n">
-        <v>62</v>
+        <v>24</v>
       </c>
       <c r="D13" t="n">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="E13" t="inlineStr">
         <is>
@@ -3764,42 +3788,42 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>[4 of Spades, 5 of Spades]</t>
+          <t>[4 of Hearts, 7 of Clubs, Queen of Hearts, 10 of Spades]</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>[2 of Diamonds, 10 of Diamonds, Jack of Hearts]</t>
+          <t>[1 of Diamonds, 10 of Diamonds]</t>
         </is>
       </c>
       <c r="C14" t="n">
-        <v>9</v>
+        <v>31</v>
       </c>
       <c r="D14" t="n">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>Win</t>
+          <t>Lose</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>[2 of Hearts, 1 of Hearts, 4 of Hearts, Jack of Diamonds, 3 of Spades]</t>
+          <t>[Jack of Diamonds, Jack of Spades]</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>[6 of Clubs, King of Spades, 2 of Clubs]</t>
+          <t>[8 of Hearts, 8 of Clubs, 1 of Hearts]</t>
         </is>
       </c>
       <c r="C15" t="n">
         <v>20</v>
       </c>
       <c r="D15" t="n">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E15" t="inlineStr">
         <is>
@@ -3810,19 +3834,19 @@
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>[Jack of Spades, 10 of Clubs, 1 of Hearts, 1 of Diamonds]</t>
+          <t>[6 of Clubs, Queen of Spades]</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>[7 of Diamonds, 7 of Spades, 9 of Hearts]</t>
+          <t>[King of Hearts, 1 of Clubs]</t>
         </is>
       </c>
       <c r="C16" t="n">
-        <v>32</v>
+        <v>16</v>
       </c>
       <c r="D16" t="n">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="E16" t="inlineStr">
         <is>
@@ -3833,30 +3857,69 @@
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>[3 of Hearts, 6 of Hearts, 8 of Hearts, 9 of Hearts, 10 of Spades]</t>
+          <t>[Queen of Hearts, Jack of Spades]</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>[6 of Spades, 1 of Clubs]</t>
+          <t>[5 of Spades, 5 of Hearts, Queen of Clubs]</t>
         </is>
       </c>
       <c r="C17" t="n">
-        <v>36</v>
+        <v>20</v>
       </c>
       <c r="D17" t="n">
+        <v>20</v>
+      </c>
+      <c r="E17" t="inlineStr">
+        <is>
+          <t>Tie</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>[3 of Clubs, 2 of Spades]</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>[10 of Diamonds, 5 of Diamonds, King of Spades]</t>
+        </is>
+      </c>
+      <c r="C18" t="n">
+        <v>5</v>
+      </c>
+      <c r="D18" t="n">
+        <v>25</v>
+      </c>
+      <c r="E18" t="inlineStr">
+        <is>
+          <t>Win</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>[10 of Hearts, 7 of Spades]</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>[9 of Clubs, 8 of Spades]</t>
+        </is>
+      </c>
+      <c r="C19" t="n">
         <v>17</v>
       </c>
-      <c r="E17" t="inlineStr">
-        <is>
-          <t>Lose</t>
-        </is>
-      </c>
-    </row>
-    <row r="18">
-      <c r="E18" t="inlineStr">
-        <is>
-          <t>% 25.00</t>
+      <c r="D19" t="n">
+        <v>17</v>
+      </c>
+      <c r="E19" t="inlineStr">
+        <is>
+          <t>Tie</t>
         </is>
       </c>
     </row>
@@ -3871,7 +3934,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E18"/>
+  <dimension ref="A1:E16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3909,65 +3972,65 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>[2 of Hearts, 5 of Hearts]</t>
+          <t>[9 of Spades, 1 of Spades]</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>[5 of Clubs, 6 of Diamonds, 8 of Spades]</t>
+          <t>[4 of Diamonds, 9 of Diamonds, 3 of Clubs, 9 of Spades]</t>
         </is>
       </c>
       <c r="C2" t="n">
-        <v>7</v>
+        <v>20</v>
       </c>
       <c r="D2" t="n">
-        <v>19</v>
+        <v>25</v>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>Lose</t>
+          <t>Win</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>[8 of Hearts, 4 of Hearts]</t>
+          <t>[6 of Hearts, Jack of Clubs]</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>[10 of Hearts, 8 of Spades]</t>
+          <t>[2 of Spades, 3 of Spades, 7 of Diamonds, Queen of Diamonds]</t>
         </is>
       </c>
       <c r="C3" t="n">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="D3" t="n">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>Lose</t>
+          <t>Win</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>[8 of Clubs, 8 of Clubs, 2 of Diamonds]</t>
+          <t>[2 of Diamonds, 10 of Spades, 3 of Clubs, Jack of Spades, 5 of Clubs, 2 of Hearts, Jack of Diamonds]</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>[3 of Spades, Queen of Spades, 7 of Hearts]</t>
+          <t>[Queen of Clubs, 4 of Clubs, 9 of Hearts]</t>
         </is>
       </c>
       <c r="C4" t="n">
-        <v>18</v>
+        <v>42</v>
       </c>
       <c r="D4" t="n">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="E4" t="inlineStr">
         <is>
@@ -3978,19 +4041,19 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>[1 of Spades, 3 of Hearts, 5 of Spades, Jack of Clubs, 5 of Diamonds, King of Clubs]</t>
+          <t>[1 of Diamonds, 6 of Clubs, Jack of Clubs, 7 of Spades, 8 of Diamonds]</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>[3 of Diamonds, 6 of Hearts, King of Diamonds]</t>
+          <t>[3 of Diamonds, Jack of Hearts, 8 of Hearts]</t>
         </is>
       </c>
       <c r="C5" t="n">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="D5" t="n">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="E5" t="inlineStr">
         <is>
@@ -4001,19 +4064,19 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>[7 of Diamonds, Jack of Diamonds, 3 of Clubs]</t>
+          <t>[King of Spades, 10 of Hearts]</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>[Queen of Diamonds, 2 of Spades, 5 of Clubs]</t>
+          <t>[5 of Clubs, 8 of Spades, King of Clubs]</t>
         </is>
       </c>
       <c r="C6" t="n">
         <v>20</v>
       </c>
       <c r="D6" t="n">
-        <v>17</v>
+        <v>23</v>
       </c>
       <c r="E6" t="inlineStr">
         <is>
@@ -4024,19 +4087,19 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>[3 of Clubs, 4 of Clubs]</t>
+          <t>[Jack of Diamonds, 7 of Diamonds]</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>[Queen of Clubs, 7 of Clubs]</t>
+          <t>[Queen of Hearts, 2 of Clubs, 1 of Spades, 8 of Hearts]</t>
         </is>
       </c>
       <c r="C7" t="n">
-        <v>7</v>
+        <v>17</v>
       </c>
       <c r="D7" t="n">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="E7" t="inlineStr">
         <is>
@@ -4047,42 +4110,42 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>[9 of Clubs, 6 of Diamonds, 7 of Clubs]</t>
+          <t>[King of Hearts, 3 of Hearts, 6 of Diamonds]</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>[5 of Hearts, King of Spades, Jack of Clubs]</t>
+          <t>[4 of Hearts, King of Diamonds, King of Spades]</t>
         </is>
       </c>
       <c r="C8" t="n">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="D8" t="n">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>Lose</t>
+          <t>Win</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>[5 of Diamonds, Jack of Spades, 10 of Diamonds]</t>
+          <t>[Queen of Diamonds, 8 of Diamonds, 6 of Hearts, 6 of Spades, 7 of Spades, 2 of Diamonds]</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>[4 of Diamonds, Queen of Diamonds, Queen of Hearts]</t>
+          <t>[King of Hearts, King of Clubs]</t>
         </is>
       </c>
       <c r="C9" t="n">
-        <v>25</v>
+        <v>39</v>
       </c>
       <c r="D9" t="n">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="E9" t="inlineStr">
         <is>
@@ -4093,42 +4156,42 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>[King of Hearts, 6 of Spades, 4 of Diamonds]</t>
+          <t>[3 of Spades, Queen of Hearts]</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>[8 of Diamonds, Queen of Clubs]</t>
+          <t>[10 of Hearts, 4 of Spades, 1 of Clubs, 5 of Diamonds]</t>
         </is>
       </c>
       <c r="C10" t="n">
+        <v>13</v>
+      </c>
+      <c r="D10" t="n">
         <v>20</v>
       </c>
-      <c r="D10" t="n">
-        <v>18</v>
-      </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>Win</t>
+          <t>Lose</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>[8 of Diamonds, King of Hearts]</t>
+          <t>[1 of Hearts, 1 of Clubs]</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>[10 of Hearts, 9 of Spades]</t>
+          <t>[10 of Clubs, 5 of Hearts, 6 of Clubs]</t>
         </is>
       </c>
       <c r="C11" t="n">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="D11" t="n">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="E11" t="inlineStr">
         <is>
@@ -4139,42 +4202,42 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>[1 of Clubs, 1 of Spades]</t>
+          <t>[5 of Spades, Jack of Spades, 3 of Diamonds]</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>[7 of Spades, 4 of Clubs, Jack of Hearts]</t>
+          <t>[2 of Spades, Queen of Spades, Jack of Hearts]</t>
         </is>
       </c>
       <c r="C12" t="n">
-        <v>12</v>
+        <v>18</v>
       </c>
       <c r="D12" t="n">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>Lose</t>
+          <t>Win</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>[4 of Spades, 9 of Clubs, 10 of Clubs, Queen of Hearts, 9 of Diamonds, King of Clubs, 1 of Diamonds, 9 of Diamonds]</t>
+          <t>[King of Diamonds, 8 of Clubs, 5 of Diamonds]</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>[10 of Spades, 2 of Spades, Queen of Spades]</t>
+          <t>[10 of Clubs, 7 of Hearts]</t>
         </is>
       </c>
       <c r="C13" t="n">
-        <v>62</v>
+        <v>23</v>
       </c>
       <c r="D13" t="n">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="E13" t="inlineStr">
         <is>
@@ -4185,42 +4248,42 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>[4 of Spades, 5 of Spades]</t>
+          <t>[6 of Spades, 5 of Spades, 5 of Hearts, 9 of Clubs]</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>[2 of Diamonds, 10 of Diamonds, Jack of Hearts]</t>
+          <t>[4 of Clubs, 9 of Diamonds, 9 of Hearts]</t>
         </is>
       </c>
       <c r="C14" t="n">
-        <v>9</v>
+        <v>25</v>
       </c>
       <c r="D14" t="n">
         <v>22</v>
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>Win</t>
+          <t>Lose</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>[2 of Hearts, 1 of Hearts, 4 of Hearts, Jack of Diamonds, 3 of Spades]</t>
+          <t>[10 of Diamonds, 7 of Clubs]</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>[6 of Clubs, King of Spades, 2 of Clubs]</t>
+          <t>[Queen of Spades, 4 of Diamonds, 2 of Clubs, 6 of Diamonds]</t>
         </is>
       </c>
       <c r="C15" t="n">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="D15" t="n">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="E15" t="inlineStr">
         <is>
@@ -4231,53 +4294,23 @@
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>[Jack of Spades, 10 of Clubs, 1 of Hearts, 1 of Diamonds]</t>
+          <t>[4 of Spades, 2 of Hearts, 8 of Clubs]</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>[7 of Diamonds, 7 of Spades, 9 of Hearts]</t>
+          <t>[3 of Hearts, 10 of Spades, Queen of Clubs]</t>
         </is>
       </c>
       <c r="C16" t="n">
-        <v>32</v>
+        <v>14</v>
       </c>
       <c r="D16" t="n">
         <v>23</v>
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>Lose</t>
-        </is>
-      </c>
-    </row>
-    <row r="17">
-      <c r="A17" t="inlineStr">
-        <is>
-          <t>[3 of Hearts, 6 of Hearts, 8 of Hearts, 9 of Hearts, 10 of Spades]</t>
-        </is>
-      </c>
-      <c r="B17" t="inlineStr">
-        <is>
-          <t>[6 of Spades, 1 of Clubs]</t>
-        </is>
-      </c>
-      <c r="C17" t="n">
-        <v>36</v>
-      </c>
-      <c r="D17" t="n">
-        <v>17</v>
-      </c>
-      <c r="E17" t="inlineStr">
-        <is>
-          <t>Lose</t>
-        </is>
-      </c>
-    </row>
-    <row r="18">
-      <c r="E18" t="inlineStr">
-        <is>
-          <t>% 25.00</t>
+          <t>Win</t>
         </is>
       </c>
     </row>
@@ -4292,7 +4325,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E18"/>
+  <dimension ref="A1:E19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -4330,16 +4363,16 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>[2 of Hearts, 5 of Hearts]</t>
+          <t>[9 of Spades, 3 of Hearts]</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>[5 of Clubs, 6 of Diamonds, 8 of Spades]</t>
+          <t>[1 of Clubs, 4 of Diamonds, 4 of Clubs]</t>
         </is>
       </c>
       <c r="C2" t="n">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="D2" t="n">
         <v>19</v>
@@ -4353,39 +4386,39 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>[8 of Hearts, 4 of Hearts]</t>
+          <t>[Queen of Diamonds, 1 of Spades]</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>[10 of Hearts, 8 of Spades]</t>
+          <t>[Jack of Hearts, 3 of Diamonds, 9 of Hearts]</t>
         </is>
       </c>
       <c r="C3" t="n">
-        <v>12</v>
+        <v>21</v>
       </c>
       <c r="D3" t="n">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>Lose</t>
+          <t>Win</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>[8 of Clubs, 8 of Clubs, 2 of Diamonds]</t>
+          <t>[5 of Clubs, 1 of Hearts]</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>[3 of Spades, Queen of Spades, 7 of Hearts]</t>
+          <t>[King of Spades, Jack of Spades]</t>
         </is>
       </c>
       <c r="C4" t="n">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="D4" t="n">
         <v>20</v>
@@ -4399,19 +4432,19 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>[1 of Spades, 3 of Hearts, 5 of Spades, Jack of Clubs, 5 of Diamonds, King of Clubs]</t>
+          <t>[2 of Clubs, 8 of Diamonds]</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>[3 of Diamonds, 6 of Hearts, King of Diamonds]</t>
+          <t>[Jack of Diamonds, Queen of Clubs]</t>
         </is>
       </c>
       <c r="C5" t="n">
-        <v>34</v>
+        <v>10</v>
       </c>
       <c r="D5" t="n">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="E5" t="inlineStr">
         <is>
@@ -4422,19 +4455,19 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>[7 of Diamonds, Jack of Diamonds, 3 of Clubs]</t>
+          <t>[10 of Clubs, 2 of Clubs, 6 of Hearts]</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>[Queen of Diamonds, 2 of Spades, 5 of Clubs]</t>
+          <t>[1 of Clubs, 2 of Hearts, 2 of Hearts, 8 of Hearts, King of Clubs]</t>
         </is>
       </c>
       <c r="C6" t="n">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="D6" t="n">
-        <v>17</v>
+        <v>23</v>
       </c>
       <c r="E6" t="inlineStr">
         <is>
@@ -4445,65 +4478,65 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>[3 of Clubs, 4 of Clubs]</t>
+          <t>[7 of Spades, 3 of Clubs]</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>[Queen of Clubs, 7 of Clubs]</t>
+          <t>[Queen of Diamonds, 6 of Clubs, King of Hearts]</t>
         </is>
       </c>
       <c r="C7" t="n">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="D7" t="n">
-        <v>17</v>
+        <v>26</v>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>Lose</t>
+          <t>Win</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>[9 of Clubs, 6 of Diamonds, 7 of Clubs]</t>
+          <t>[10 of Clubs, 5 of Spades]</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>[5 of Hearts, King of Spades, Jack of Clubs]</t>
+          <t>[5 of Diamonds, King of Clubs, Jack of Clubs]</t>
         </is>
       </c>
       <c r="C8" t="n">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="D8" t="n">
         <v>25</v>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>Lose</t>
+          <t>Win</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>[5 of Diamonds, Jack of Spades, 10 of Diamonds]</t>
+          <t>[6 of Spades, 6 of Clubs]</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>[4 of Diamonds, Queen of Diamonds, Queen of Hearts]</t>
+          <t>[6 of Diamonds, 4 of Diamonds, Queen of Clubs]</t>
         </is>
       </c>
       <c r="C9" t="n">
-        <v>25</v>
+        <v>12</v>
       </c>
       <c r="D9" t="n">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="E9" t="inlineStr">
         <is>
@@ -4514,19 +4547,19 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>[King of Hearts, 6 of Spades, 4 of Diamonds]</t>
+          <t>[2 of Diamonds, 2 of Spades, 3 of Spades]</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>[8 of Diamonds, Queen of Clubs]</t>
+          <t>[Queen of Spades, 6 of Hearts, 7 of Spades]</t>
         </is>
       </c>
       <c r="C10" t="n">
-        <v>20</v>
+        <v>7</v>
       </c>
       <c r="D10" t="n">
-        <v>18</v>
+        <v>23</v>
       </c>
       <c r="E10" t="inlineStr">
         <is>
@@ -4537,39 +4570,39 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>[8 of Diamonds, King of Hearts]</t>
+          <t>[5 of Hearts, Queen of Hearts]</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>[10 of Hearts, 9 of Spades]</t>
+          <t>[4 of Spades, 7 of Diamonds, 4 of Clubs, 8 of Clubs]</t>
         </is>
       </c>
       <c r="C11" t="n">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="D11" t="n">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>Lose</t>
+          <t>Win</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>[1 of Clubs, 1 of Spades]</t>
+          <t>[3 of Spades, 2 of Spades, 9 of Diamonds, 5 of Hearts, 1 of Spades, 7 of Clubs]</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>[7 of Spades, 4 of Clubs, Jack of Hearts]</t>
+          <t>[Queen of Spades, 1 of Hearts]</t>
         </is>
       </c>
       <c r="C12" t="n">
-        <v>12</v>
+        <v>27</v>
       </c>
       <c r="D12" t="n">
         <v>21</v>
@@ -4583,19 +4616,19 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>[4 of Spades, 9 of Clubs, 10 of Clubs, Queen of Hearts, 9 of Diamonds, King of Clubs, 1 of Diamonds, 9 of Diamonds]</t>
+          <t>[6 of Spades, 9 of Clubs]</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>[10 of Spades, 2 of Spades, Queen of Spades]</t>
+          <t>[8 of Spades, 8 of Diamonds, 1 of Diamonds]</t>
         </is>
       </c>
       <c r="C13" t="n">
-        <v>62</v>
+        <v>15</v>
       </c>
       <c r="D13" t="n">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="E13" t="inlineStr">
         <is>
@@ -4606,65 +4639,65 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>[4 of Spades, 5 of Spades]</t>
+          <t>[6 of Diamonds, 7 of Hearts, 5 of Clubs, 7 of Diamonds]</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>[2 of Diamonds, 10 of Diamonds, Jack of Hearts]</t>
+          <t>[2 of Diamonds, 10 of Spades, King of Diamonds]</t>
         </is>
       </c>
       <c r="C14" t="n">
-        <v>9</v>
+        <v>25</v>
       </c>
       <c r="D14" t="n">
         <v>22</v>
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>Win</t>
+          <t>Lose</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>[2 of Hearts, 1 of Hearts, 4 of Hearts, Jack of Diamonds, 3 of Spades]</t>
+          <t>[Queen of Hearts, 4 of Hearts]</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>[6 of Clubs, King of Spades, 2 of Clubs]</t>
+          <t>[10 of Diamonds, 9 of Clubs]</t>
         </is>
       </c>
       <c r="C15" t="n">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="D15" t="n">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>Win</t>
+          <t>Lose</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>[Jack of Spades, 10 of Clubs, 1 of Hearts, 1 of Diamonds]</t>
+          <t>[4 of Spades, 3 of Hearts]</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>[7 of Diamonds, 7 of Spades, 9 of Hearts]</t>
+          <t>[4 of Hearts, 7 of Hearts, 10 of Hearts]</t>
         </is>
       </c>
       <c r="C16" t="n">
-        <v>32</v>
+        <v>7</v>
       </c>
       <c r="D16" t="n">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="E16" t="inlineStr">
         <is>
@@ -4675,19 +4708,19 @@
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>[3 of Hearts, 6 of Hearts, 8 of Hearts, 9 of Hearts, 10 of Spades]</t>
+          <t>[9 of Spades, 9 of Hearts]</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>[6 of Spades, 1 of Clubs]</t>
+          <t>[10 of Spades, 10 of Diamonds]</t>
         </is>
       </c>
       <c r="C17" t="n">
-        <v>36</v>
+        <v>18</v>
       </c>
       <c r="D17" t="n">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="E17" t="inlineStr">
         <is>
@@ -4696,9 +4729,48 @@
       </c>
     </row>
     <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>[8 of Spades, 8 of Hearts, King of Spades]</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>[Jack of Diamonds, King of Hearts]</t>
+        </is>
+      </c>
+      <c r="C18" t="n">
+        <v>26</v>
+      </c>
+      <c r="D18" t="n">
+        <v>20</v>
+      </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>% 25.00</t>
+          <t>Lose</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>[5 of Diamonds, Jack of Spades]</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>[Jack of Hearts, 9 of Diamonds]</t>
+        </is>
+      </c>
+      <c r="C19" t="n">
+        <v>15</v>
+      </c>
+      <c r="D19" t="n">
+        <v>19</v>
+      </c>
+      <c r="E19" t="inlineStr">
+        <is>
+          <t>Lose</t>
         </is>
       </c>
     </row>

</xml_diff>